<commit_message>
Created logic for building the alignments
</commit_message>
<xml_diff>
--- a/tabular/lassa-data.xlsx
+++ b/tabular/lassa-data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/Lassa-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E51023-A3CF-F649-8836-DEF7712CDC1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9964C088-3386-DD45-8859-F1F1E4DCA884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sequences.txt" sheetId="1" r:id="rId1"/>
+    <sheet name="lassa-data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12667" uniqueCount="2414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12673" uniqueCount="2414">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -7668,7 +7668,7 @@
   <dimension ref="A1:H1937"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -58012,9 +58012,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1937" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1937" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1937" t="s">
         <v>2413</v>
+      </c>
+      <c r="B1937" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1937" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1937" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1937" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1937" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1937" t="b">
+        <v>1</v>
+      </c>
+      <c r="H1937" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added missing segment data. Alignment select member clauses modified
</commit_message>
<xml_diff>
--- a/tabular/lassa-data.xlsx
+++ b/tabular/lassa-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/epidemiology/Lassa-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61C7690-B635-0448-BC74-DDE7EDB6352A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66CDEA8-F5D6-5C4D-AA59-FB0B7DC5BFD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="560" windowWidth="16880" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6280" yWindow="460" windowWidth="16880" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lassa-data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12885" uniqueCount="2446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12884" uniqueCount="2447">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -7363,6 +7363,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Soromba</t>
   </si>
 </sst>
 </file>
@@ -7800,8 +7803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1967"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="D139" sqref="A1:H1967"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7848,7 +7851,7 @@
         <v>10888638</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -7874,7 +7877,7 @@
         <v>10888638</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E3" s="1">
         <v>803213</v>
@@ -7900,7 +7903,7 @@
         <v>10888638</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -7926,7 +7929,7 @@
         <v>10888638</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
@@ -7952,7 +7955,7 @@
         <v>10888638</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -7978,7 +7981,7 @@
         <v>10888638</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>15</v>
@@ -8004,7 +8007,7 @@
         <v>10888638</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
@@ -8030,7 +8033,7 @@
         <v>10888638</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>19</v>
@@ -8056,7 +8059,7 @@
         <v>10888638</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>21</v>
@@ -8082,7 +8085,7 @@
         <v>10888638</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>23</v>
@@ -8108,7 +8111,7 @@
         <v>10888638</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>25</v>
@@ -8134,7 +8137,7 @@
         <v>10888638</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>27</v>
@@ -8160,7 +8163,7 @@
         <v>10888638</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>29</v>
@@ -8186,7 +8189,7 @@
         <v>10888638</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>31</v>
@@ -8212,7 +8215,7 @@
         <v>10888638</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>33</v>
@@ -8238,7 +8241,7 @@
         <v>10888638</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>35</v>
@@ -8264,7 +8267,7 @@
         <v>10888638</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>37</v>
@@ -8290,7 +8293,7 @@
         <v>10888638</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>39</v>
@@ -8316,7 +8319,7 @@
         <v>10888638</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>41</v>
@@ -8342,7 +8345,7 @@
         <v>10888638</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>43</v>
@@ -8368,7 +8371,7 @@
         <v>10888638</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>45</v>
@@ -8394,7 +8397,7 @@
         <v>10888638</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>47</v>
@@ -8420,7 +8423,7 @@
         <v>10888638</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>49</v>
@@ -8446,7 +8449,7 @@
         <v>10888638</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>51</v>
@@ -8472,7 +8475,7 @@
         <v>10888638</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>53</v>
@@ -8498,7 +8501,7 @@
         <v>10888638</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>55</v>
@@ -8524,7 +8527,7 @@
         <v>10888638</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>57</v>
@@ -8550,7 +8553,7 @@
         <v>10888638</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>59</v>
@@ -8576,7 +8579,7 @@
         <v>10888638</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>61</v>
@@ -8602,7 +8605,7 @@
         <v>10888638</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>63</v>
@@ -8628,7 +8631,7 @@
         <v>10888638</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>65</v>
@@ -8654,7 +8657,7 @@
         <v>10888638</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>67</v>
@@ -8680,7 +8683,7 @@
         <v>10888638</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>69</v>
@@ -8706,7 +8709,7 @@
         <v>10888638</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>71</v>
@@ -8732,7 +8735,7 @@
         <v>10888638</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>73</v>
@@ -8758,7 +8761,7 @@
         <v>10888638</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>75</v>
@@ -8784,7 +8787,7 @@
         <v>10888638</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>77</v>
@@ -8810,7 +8813,7 @@
         <v>10888638</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>79</v>
@@ -8836,7 +8839,7 @@
         <v>10888638</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>81</v>
@@ -8862,7 +8865,7 @@
         <v>10888638</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>83</v>
@@ -8888,7 +8891,7 @@
         <v>10888638</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>85</v>
@@ -8914,7 +8917,7 @@
         <v>10888638</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>87</v>
@@ -8940,7 +8943,7 @@
         <v>10888638</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>89</v>
@@ -8966,7 +8969,7 @@
         <v>10888638</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>91</v>
@@ -8992,7 +8995,7 @@
         <v>10888638</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>93</v>
@@ -9018,7 +9021,7 @@
         <v>10888638</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>95</v>
@@ -9044,7 +9047,7 @@
         <v>10888638</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>97</v>
@@ -9070,7 +9073,7 @@
         <v>10888638</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>99</v>
@@ -9096,7 +9099,7 @@
         <v>10888638</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>101</v>
@@ -9122,7 +9125,7 @@
         <v>10888638</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>103</v>
@@ -9148,7 +9151,7 @@
         <v>10888638</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>105</v>
@@ -9174,7 +9177,7 @@
         <v>10888638</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>107</v>
@@ -9200,7 +9203,7 @@
         <v>10888638</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>109</v>
@@ -9226,7 +9229,7 @@
         <v>10888638</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>111</v>
@@ -9252,7 +9255,7 @@
         <v>10888638</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>113</v>
@@ -9278,7 +9281,7 @@
         <v>10888638</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>115</v>
@@ -9304,7 +9307,7 @@
         <v>10998376</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>117</v>
@@ -9330,7 +9333,7 @@
         <v>11443561</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>119</v>
@@ -9356,7 +9359,7 @@
         <v>14972544</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>119</v>
@@ -9382,7 +9385,7 @@
         <v>2445</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>2445</v>
@@ -9408,7 +9411,7 @@
         <v>7883875</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>2445</v>
@@ -9434,7 +9437,7 @@
         <v>7883875</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>2445</v>
@@ -9460,7 +9463,7 @@
         <v>7883875</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>2445</v>
@@ -9486,7 +9489,7 @@
         <v>7883875</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>2445</v>
@@ -9512,7 +9515,7 @@
         <v>7883875</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>2445</v>
@@ -9538,7 +9541,7 @@
         <v>7883875</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>2445</v>
@@ -9564,7 +9567,7 @@
         <v>14972544</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>117</v>
@@ -9590,7 +9593,7 @@
         <v>14972544</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>134</v>
@@ -9642,7 +9645,7 @@
         <v>14698659</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>138</v>
@@ -9668,7 +9671,7 @@
         <v>17905372</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>140</v>
@@ -9694,7 +9697,7 @@
         <v>17905372</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>142</v>
@@ -9720,7 +9723,7 @@
         <v>17905372</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>144</v>
@@ -9746,7 +9749,7 @@
         <v>17905372</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>146</v>
@@ -9772,7 +9775,7 @@
         <v>17905372</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>148</v>
@@ -9798,7 +9801,7 @@
         <v>17905372</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>150</v>
@@ -9824,7 +9827,7 @@
         <v>2445</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>152</v>
@@ -9876,7 +9879,7 @@
         <v>2445</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>138</v>
@@ -9928,7 +9931,7 @@
         <v>2445</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>157</v>
@@ -10058,7 +10061,7 @@
         <v>17905372</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>166</v>
@@ -10084,7 +10087,7 @@
         <v>17905372</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>91</v>
@@ -10110,7 +10113,7 @@
         <v>17905372</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>27</v>
@@ -10136,7 +10139,7 @@
         <v>17905372</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>9</v>
@@ -10162,7 +10165,7 @@
         <v>17905372</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>171</v>
@@ -10188,7 +10191,7 @@
         <v>2445</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>2445</v>
@@ -10214,7 +10217,7 @@
         <v>2445</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>2445</v>
@@ -10240,7 +10243,7 @@
         <v>2445</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>2445</v>
@@ -10266,7 +10269,7 @@
         <v>2445</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>2445</v>
@@ -10292,7 +10295,7 @@
         <v>2445</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>2445</v>
@@ -10318,7 +10321,7 @@
         <v>2445</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>2445</v>
@@ -10396,7 +10399,7 @@
         <v>17326956</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>2445</v>
@@ -10422,7 +10425,7 @@
         <v>17326956</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>2445</v>
@@ -10448,7 +10451,7 @@
         <v>17326956</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>2445</v>
@@ -10474,7 +10477,7 @@
         <v>17326956</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>2445</v>
@@ -10500,7 +10503,7 @@
         <v>17326956</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>2445</v>
@@ -10526,7 +10529,7 @@
         <v>17326956</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>2445</v>
@@ -10552,7 +10555,7 @@
         <v>17326956</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>2445</v>
@@ -10578,7 +10581,7 @@
         <v>17326956</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>2445</v>
@@ -10604,7 +10607,7 @@
         <v>17326956</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>2445</v>
@@ -10630,7 +10633,7 @@
         <v>17326956</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>2445</v>
@@ -10656,7 +10659,7 @@
         <v>17326956</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>2445</v>
@@ -10682,7 +10685,7 @@
         <v>17326956</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>2445</v>
@@ -10708,7 +10711,7 @@
         <v>17326956</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>2445</v>
@@ -10734,7 +10737,7 @@
         <v>17326956</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>2445</v>
@@ -10760,7 +10763,7 @@
         <v>17326956</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>2445</v>
@@ -10786,7 +10789,7 @@
         <v>17326956</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>2445</v>
@@ -10812,7 +10815,7 @@
         <v>17326956</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>2445</v>
@@ -10838,7 +10841,7 @@
         <v>17326956</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>2445</v>
@@ -10864,7 +10867,7 @@
         <v>17326956</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>2445</v>
@@ -10890,7 +10893,7 @@
         <v>17326956</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>2445</v>
@@ -10916,7 +10919,7 @@
         <v>17326956</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>2445</v>
@@ -10942,7 +10945,7 @@
         <v>17326956</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>2445</v>
@@ -10968,7 +10971,7 @@
         <v>17326956</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>2445</v>
@@ -10994,7 +10997,7 @@
         <v>17326956</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>2445</v>
@@ -11020,7 +11023,7 @@
         <v>17326956</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>2445</v>
@@ -11046,7 +11049,7 @@
         <v>17326956</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>2445</v>
@@ -11072,7 +11075,7 @@
         <v>17326956</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>2445</v>
@@ -11098,7 +11101,7 @@
         <v>17326956</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>2445</v>
@@ -11124,7 +11127,7 @@
         <v>17326956</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>2445</v>
@@ -11150,7 +11153,7 @@
         <v>17326956</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>2445</v>
@@ -11176,7 +11179,7 @@
         <v>17326956</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>2445</v>
@@ -11202,7 +11205,7 @@
         <v>17326956</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>2445</v>
@@ -11228,7 +11231,7 @@
         <v>17326956</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>2445</v>
@@ -11254,10 +11257,10 @@
         <v>2445</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>2445</v>
+        <v>2446</v>
       </c>
       <c r="F133" s="1">
         <v>873</v>
@@ -11280,7 +11283,7 @@
         <v>21880754</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>117</v>
@@ -11306,7 +11309,7 @@
         <v>21880754</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>117</v>
@@ -32340,7 +32343,7 @@
         <v>27140942</v>
       </c>
       <c r="D944" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E944" s="1" t="s">
         <v>1392</v>
@@ -32366,7 +32369,7 @@
         <v>27140942</v>
       </c>
       <c r="D945" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E945" s="1" t="s">
         <v>1394</v>
@@ -32392,7 +32395,7 @@
         <v>27140942</v>
       </c>
       <c r="D946" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E946" s="1" t="s">
         <v>1396</v>
@@ -32418,7 +32421,7 @@
         <v>27140942</v>
       </c>
       <c r="D947" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E947" s="1" t="s">
         <v>1398</v>
@@ -32444,7 +32447,7 @@
         <v>27140942</v>
       </c>
       <c r="D948" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E948" s="1" t="s">
         <v>1400</v>
@@ -32470,7 +32473,7 @@
         <v>27140942</v>
       </c>
       <c r="D949" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E949" s="1" t="s">
         <v>1402</v>
@@ -32496,7 +32499,7 @@
         <v>27140942</v>
       </c>
       <c r="D950" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E950" s="1" t="s">
         <v>1404</v>
@@ -32522,7 +32525,7 @@
         <v>27140942</v>
       </c>
       <c r="D951" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E951" s="1" t="s">
         <v>1406</v>
@@ -32548,7 +32551,7 @@
         <v>27140942</v>
       </c>
       <c r="D952" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E952" s="1" t="s">
         <v>1408</v>
@@ -32574,7 +32577,7 @@
         <v>27140942</v>
       </c>
       <c r="D953" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E953" s="1" t="s">
         <v>1411</v>
@@ -32600,7 +32603,7 @@
         <v>27140942</v>
       </c>
       <c r="D954" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E954" s="1" t="s">
         <v>1392</v>
@@ -32626,7 +32629,7 @@
         <v>27140942</v>
       </c>
       <c r="D955" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E955" s="1" t="s">
         <v>1394</v>
@@ -32652,7 +32655,7 @@
         <v>27140942</v>
       </c>
       <c r="D956" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E956" s="1" t="s">
         <v>1396</v>
@@ -32678,7 +32681,7 @@
         <v>27140942</v>
       </c>
       <c r="D957" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E957" s="1" t="s">
         <v>1398</v>
@@ -32704,7 +32707,7 @@
         <v>27140942</v>
       </c>
       <c r="D958" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E958" s="1" t="s">
         <v>1400</v>
@@ -32730,7 +32733,7 @@
         <v>27140942</v>
       </c>
       <c r="D959" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E959" s="1" t="s">
         <v>1402</v>
@@ -32756,7 +32759,7 @@
         <v>27140942</v>
       </c>
       <c r="D960" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E960" s="1" t="s">
         <v>1404</v>
@@ -32782,7 +32785,7 @@
         <v>27140942</v>
       </c>
       <c r="D961" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E961" s="1" t="s">
         <v>1406</v>
@@ -32808,7 +32811,7 @@
         <v>27140942</v>
       </c>
       <c r="D962" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E962" s="1" t="s">
         <v>1408</v>
@@ -32834,7 +32837,7 @@
         <v>27140942</v>
       </c>
       <c r="D963" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E963" s="1" t="s">
         <v>1411</v>
@@ -32860,7 +32863,7 @@
         <v>27140942</v>
       </c>
       <c r="D964" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E964" s="1" t="s">
         <v>1423</v>
@@ -32886,7 +32889,7 @@
         <v>27140942</v>
       </c>
       <c r="D965" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E965" s="1" t="s">
         <v>1425</v>
@@ -32912,7 +32915,7 @@
         <v>27140942</v>
       </c>
       <c r="D966" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E966" s="1" t="s">
         <v>1427</v>
@@ -32938,7 +32941,7 @@
         <v>27140942</v>
       </c>
       <c r="D967" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E967" s="1" t="s">
         <v>1429</v>
@@ -32964,7 +32967,7 @@
         <v>27140942</v>
       </c>
       <c r="D968" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E968" s="1" t="s">
         <v>1423</v>
@@ -32990,7 +32993,7 @@
         <v>27140942</v>
       </c>
       <c r="D969" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E969" s="1" t="s">
         <v>1425</v>
@@ -33016,7 +33019,7 @@
         <v>27140942</v>
       </c>
       <c r="D970" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E970" s="1" t="s">
         <v>1427</v>
@@ -33042,7 +33045,7 @@
         <v>27140942</v>
       </c>
       <c r="D971" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E971" s="1" t="s">
         <v>1429</v>
@@ -34628,7 +34631,7 @@
         <v>26196447</v>
       </c>
       <c r="D1032" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E1032" s="1">
         <v>124</v>
@@ -34654,7 +34657,7 @@
         <v>26196447</v>
       </c>
       <c r="D1033" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E1033" s="1">
         <v>127</v>
@@ -34680,7 +34683,7 @@
         <v>26196447</v>
       </c>
       <c r="D1034" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E1034" s="1">
         <v>132</v>
@@ -34706,7 +34709,7 @@
         <v>26196447</v>
       </c>
       <c r="D1035" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E1035" s="1">
         <v>139</v>
@@ -34732,7 +34735,7 @@
         <v>2445</v>
       </c>
       <c r="D1036" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E1036" s="1" t="s">
         <v>2445</v>
@@ -34836,16 +34839,13 @@
         <v>2445</v>
       </c>
       <c r="D1040" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1040" s="1" t="s">
         <v>2445</v>
       </c>
       <c r="F1040" s="1">
         <v>263</v>
-      </c>
-      <c r="G1040" s="1" t="s">
-        <v>2445</v>
       </c>
       <c r="H1040" s="1" t="s">
         <v>2407</v>
@@ -34862,7 +34862,7 @@
         <v>2445</v>
       </c>
       <c r="D1041" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1041" s="1" t="s">
         <v>2445</v>
@@ -34888,7 +34888,7 @@
         <v>2445</v>
       </c>
       <c r="D1042" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1042" s="1" t="s">
         <v>2445</v>
@@ -34914,7 +34914,7 @@
         <v>2445</v>
       </c>
       <c r="D1043" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1043" s="1" t="s">
         <v>2445</v>
@@ -34940,7 +34940,7 @@
         <v>2445</v>
       </c>
       <c r="D1044" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1044" s="1" t="s">
         <v>2445</v>
@@ -34966,7 +34966,7 @@
         <v>2445</v>
       </c>
       <c r="D1045" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1045" s="1" t="s">
         <v>2445</v>
@@ -34992,7 +34992,7 @@
         <v>2445</v>
       </c>
       <c r="D1046" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1046" s="1" t="s">
         <v>2445</v>
@@ -35018,7 +35018,7 @@
         <v>2445</v>
       </c>
       <c r="D1047" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1047" s="1" t="s">
         <v>2445</v>
@@ -35044,7 +35044,7 @@
         <v>2445</v>
       </c>
       <c r="D1048" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1048" s="1" t="s">
         <v>2445</v>
@@ -35070,7 +35070,7 @@
         <v>2445</v>
       </c>
       <c r="D1049" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1049" s="1" t="s">
         <v>2445</v>
@@ -35096,7 +35096,7 @@
         <v>2445</v>
       </c>
       <c r="D1050" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1050" s="1" t="s">
         <v>2445</v>
@@ -35122,7 +35122,7 @@
         <v>2445</v>
       </c>
       <c r="D1051" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1051" s="1" t="s">
         <v>2445</v>
@@ -35148,7 +35148,7 @@
         <v>2445</v>
       </c>
       <c r="D1052" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1052" s="1" t="s">
         <v>2445</v>
@@ -35174,7 +35174,7 @@
         <v>2445</v>
       </c>
       <c r="D1053" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1053" s="1" t="s">
         <v>2445</v>
@@ -35200,7 +35200,7 @@
         <v>2445</v>
       </c>
       <c r="D1054" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1054" s="1" t="s">
         <v>2445</v>
@@ -41206,7 +41206,7 @@
         <v>2445</v>
       </c>
       <c r="D1285" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1285" s="1" t="s">
         <v>2445</v>
@@ -41232,7 +41232,7 @@
         <v>2445</v>
       </c>
       <c r="D1286" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1286" s="1" t="s">
         <v>2445</v>
@@ -41258,7 +41258,7 @@
         <v>2445</v>
       </c>
       <c r="D1287" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1287" s="1" t="s">
         <v>2445</v>
@@ -41284,7 +41284,7 @@
         <v>2445</v>
       </c>
       <c r="D1288" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1288" s="1" t="s">
         <v>2445</v>
@@ -41310,7 +41310,7 @@
         <v>2445</v>
       </c>
       <c r="D1289" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1289" s="1" t="s">
         <v>2445</v>
@@ -41336,7 +41336,7 @@
         <v>2445</v>
       </c>
       <c r="D1290" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1290" s="1" t="s">
         <v>2445</v>
@@ -41362,7 +41362,7 @@
         <v>2445</v>
       </c>
       <c r="D1291" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1291" s="1" t="s">
         <v>2445</v>
@@ -41388,7 +41388,7 @@
         <v>2445</v>
       </c>
       <c r="D1292" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1292" s="1" t="s">
         <v>2445</v>
@@ -41414,7 +41414,7 @@
         <v>2445</v>
       </c>
       <c r="D1293" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1293" s="1" t="s">
         <v>2445</v>
@@ -41440,7 +41440,7 @@
         <v>2445</v>
       </c>
       <c r="D1294" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1294" s="1" t="s">
         <v>2445</v>
@@ -41466,7 +41466,7 @@
         <v>2445</v>
       </c>
       <c r="D1295" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1295" s="1" t="s">
         <v>2445</v>
@@ -41492,7 +41492,7 @@
         <v>2445</v>
       </c>
       <c r="D1296" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1296" s="1" t="s">
         <v>2445</v>
@@ -41518,7 +41518,7 @@
         <v>2445</v>
       </c>
       <c r="D1297" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1297" s="1" t="s">
         <v>2445</v>
@@ -41544,7 +41544,7 @@
         <v>2445</v>
       </c>
       <c r="D1298" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1298" s="1" t="s">
         <v>2445</v>
@@ -41570,7 +41570,7 @@
         <v>2445</v>
       </c>
       <c r="D1299" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1299" s="1" t="s">
         <v>2445</v>
@@ -41596,7 +41596,7 @@
         <v>2445</v>
       </c>
       <c r="D1300" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1300" s="1" t="s">
         <v>2445</v>
@@ -41622,7 +41622,7 @@
         <v>2445</v>
       </c>
       <c r="D1301" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1301" s="1" t="s">
         <v>2445</v>
@@ -41648,7 +41648,7 @@
         <v>2445</v>
       </c>
       <c r="D1302" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1302" s="1" t="s">
         <v>2445</v>
@@ -57976,7 +57976,7 @@
         <v>9049403</v>
       </c>
       <c r="D1930" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E1930" s="1" t="s">
         <v>138</v>
@@ -58002,7 +58002,7 @@
         <v>9281522</v>
       </c>
       <c r="D1931" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E1931" s="1" t="s">
         <v>2445</v>
@@ -58028,7 +58028,7 @@
         <v>2445</v>
       </c>
       <c r="D1932" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E1932" s="1" t="s">
         <v>2445</v>
@@ -58054,7 +58054,7 @@
         <v>9417890</v>
       </c>
       <c r="D1933" s="1" t="s">
-        <v>2445</v>
+        <v>121</v>
       </c>
       <c r="E1933" s="1" t="s">
         <v>6</v>
@@ -58080,7 +58080,7 @@
         <v>2042397</v>
       </c>
       <c r="D1934" s="1" t="s">
-        <v>2445</v>
+        <v>136</v>
       </c>
       <c r="E1934" s="1" t="s">
         <v>2398</v>

</xml_diff>